<commit_message>
modify to handle review/process doc
</commit_message>
<xml_diff>
--- a/static/upload/test3.xlsx
+++ b/static/upload/test3.xlsx
@@ -507,14 +507,14 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>QJlMYhilW4lJTBKJk2YpIMPnYmPr2Bvsvj2sqJT0CslF77YAqPhC3xwex0CUdjYbi</t>
+          <t>Ahmad Faizal bin Ramli</t>
         </is>
       </c>
       <c r="B2" t="inlineStr"/>
       <c r="C2" t="inlineStr"/>
       <c r="D2" t="inlineStr">
         <is>
-          <t>xBl_L5l4I887F6noXweA-ZwoF2y67nKFmPZ_4ifs2mc=7</t>
+          <t>900101-14-5677</t>
         </is>
       </c>
       <c r="E2" t="inlineStr"/>
@@ -535,12 +535,12 @@
       </c>
       <c r="I2" t="inlineStr">
         <is>
-          <t>Tsgfi376p7p7a9nzmbsrpcsV-IgBJlaMBmK22kHZSGL5hX3z0boWmTOjuy-yvkSLm</t>
+          <t>faizal.ramli@gmail.com</t>
         </is>
       </c>
       <c r="J2" t="inlineStr">
         <is>
-          <t>TV53ukKvBx7cJy8bwH8ZulU5TN9x6vxGcI7x9RpqCyM=9</t>
+          <t>012-3456789</t>
         </is>
       </c>
       <c r="K2" t="inlineStr">
@@ -560,14 +560,14 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>2njB-stjmaT6m01Wxq9i1u6RCb8ZE6GU-Xg5jwXCVoc=n</t>
+          <t>Lim Wei Chen</t>
         </is>
       </c>
       <c r="B3" t="inlineStr"/>
       <c r="C3" t="inlineStr"/>
       <c r="D3" t="inlineStr">
         <is>
-          <t>HqfmNF1ZKskApsFVgHnoN9H3RlAB43QCI5APlxXYL0w=4</t>
+          <t>880505-08-1234</t>
         </is>
       </c>
       <c r="E3" t="inlineStr"/>
@@ -588,12 +588,12 @@
       </c>
       <c r="I3" t="inlineStr">
         <is>
-          <t>mXZuayvu8IYoy2nTJtY4UT0HaaJ1er2MhyzkWn2tlFUPPedSmRambyXywMos9zGUm</t>
+          <t>wei.chen@outlook.com</t>
         </is>
       </c>
       <c r="J3" t="inlineStr">
         <is>
-          <t>FrGEdfOTGZrI6rgwjJgHiOC0sEYSnbXHBxVdc02Qy7E=8</t>
+          <t>+6016 2345678</t>
         </is>
       </c>
       <c r="K3" t="inlineStr">
@@ -613,14 +613,14 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>_L-lCI3FCg8BQkhRz_Hs4n7Ks6wVFtoh_SSnzMJMiiXoxjAZnFFCdu2bwNBnUgKHy</t>
+          <t>A/P Suguna Muniandy</t>
         </is>
       </c>
       <c r="B4" t="inlineStr"/>
       <c r="C4" t="inlineStr"/>
       <c r="D4" t="inlineStr">
         <is>
-          <t>u7LINOmKNK7sDlNwiNzzxUYQpZGOkZuypXFhUpgiHwI=6</t>
+          <t>850321-10-3456</t>
         </is>
       </c>
       <c r="E4" t="inlineStr"/>
@@ -641,12 +641,12 @@
       </c>
       <c r="I4" t="inlineStr">
         <is>
-          <t>1j0fiGMMwfq8e4wk31IT32WIVgqYl7hf2oLLbr9bZSwGauxnpVP-jw8i5RA0o-WIm</t>
+          <t>suguna.m@gmail.com</t>
         </is>
       </c>
       <c r="J4" t="inlineStr">
         <is>
-          <t>VDTMApE5CJCmMropvD5sHR-T52cmuAJi9RRQM1eDuWI=3</t>
+          <t>019 9876543</t>
         </is>
       </c>
       <c r="K4" t="inlineStr">
@@ -666,14 +666,14 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>6WrgNFc-OJT53a-siZWbPR-3JXE4ZIRDZ4mnDBetmk68XvRqc4eUosFq_J0G-Q3-g</t>
+          <t>Dayang Nurul binti Awang</t>
         </is>
       </c>
       <c r="B5" t="inlineStr"/>
       <c r="C5" t="inlineStr"/>
       <c r="D5" t="inlineStr">
         <is>
-          <t>JtZ9SOJaeMu05vK8uwB6A6CtbKvyQkqeCUx7YJAgLno=2</t>
+          <t>920212-13-2222</t>
         </is>
       </c>
       <c r="E5" t="inlineStr"/>
@@ -694,12 +694,12 @@
       </c>
       <c r="I5" t="inlineStr">
         <is>
-          <t>X1BwkQfapcTnyX3xhLfvsYmX1H3zAvc8dlTWhgI2IGCh5p6I2BP9Z7gT6KlVTYOGm</t>
+          <t>dayang.awang@yahoo.com</t>
         </is>
       </c>
       <c r="J5" t="inlineStr">
         <is>
-          <t>C7htg_9vWD0QWef0r63phPwWyo-lT1VNs-iX-NVqVdM=3</t>
+          <t>014-2223333</t>
         </is>
       </c>
       <c r="K5" t="inlineStr">
@@ -719,14 +719,14 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>tmkK1vNAAMtEsMJfbQAqhD3IED2IiM5LVOMnJx-AgC5PFy3bF_-i3Dm1rpsp97a3g</t>
+          <t>Richard Anak Balang</t>
         </is>
       </c>
       <c r="B6" t="inlineStr"/>
       <c r="C6" t="inlineStr"/>
       <c r="D6" t="inlineStr">
         <is>
-          <t>QaWdadofRUrntomM1WoRyNFL58T_dDWiagExJSmKyng=6</t>
+          <t>790715-52-9876</t>
         </is>
       </c>
       <c r="E6" t="inlineStr"/>
@@ -747,7 +747,7 @@
       </c>
       <c r="I6" t="inlineStr">
         <is>
-          <t>TsVUWVtHU9dR9Vj5r3Rc1dgaCdEwb-XNWodPL1rksbZ7hZxc7k3wMKSuzLajSvjjm</t>
+          <t>richard.balang@gmail.com</t>
         </is>
       </c>
       <c r="J6" t="inlineStr"/>
@@ -768,14 +768,14 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>HnrnbfGTQdlt-jGIw10TUyWXPCIKUSGXEl-WiL2cIRQ=f</t>
+          <t>Nurul Aina Yusof</t>
         </is>
       </c>
       <c r="B7" t="inlineStr"/>
       <c r="C7" t="inlineStr"/>
       <c r="D7" t="inlineStr">
         <is>
-          <t>gld13poxPPr0i3Y1pMs00LDtLK_sJkfZycqAsMZEtgY=7</t>
+          <t>030202-03-4567</t>
         </is>
       </c>
       <c r="E7" t="inlineStr"/>
@@ -796,12 +796,12 @@
       </c>
       <c r="I7" t="inlineStr">
         <is>
-          <t>lpKznpE6WmbtiDDrttqIONQvx6yXW3ngiSMsx5893MDiyFB8wzMpq0Pmqbn9kaxCm</t>
+          <t>nurul.aina@yahoo.com</t>
         </is>
       </c>
       <c r="J7" t="inlineStr">
         <is>
-          <t>VW_e9dplsN2Xqmi8CXm5Xnh4Pyaxy5R7gsRwVMkSoOQ=6</t>
+          <t>017-3344556</t>
         </is>
       </c>
       <c r="K7" t="inlineStr">
@@ -821,7 +821,7 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>z4T0lyTSiyqA-g31Vuf2zVDGHZMm-eO0R8Ke4gtWd9s=h</t>
+          <t>John Smith</t>
         </is>
       </c>
       <c r="B8" t="inlineStr"/>
@@ -829,7 +829,7 @@
       <c r="D8" t="inlineStr"/>
       <c r="E8" t="inlineStr">
         <is>
-          <t>0q-Kfflo8fTtm8mv-VP7f9U0r0rqBuxjE0mVjRj9UJM=8</t>
+          <t>A12345678</t>
         </is>
       </c>
       <c r="F8" t="inlineStr">
@@ -849,12 +849,12 @@
       </c>
       <c r="I8" t="inlineStr">
         <is>
-          <t>eIKIE-x4oEhzCrxLyUGtImEFeqbz2Yt-FqNx_5YuTFJYf2TbnqPAGYmY-PI40Pdgm</t>
+          <t>johnsmith@domain.com</t>
         </is>
       </c>
       <c r="J8" t="inlineStr">
         <is>
-          <t>_aaQMxIR5CHsTIlJwBEhQCPYhgrT15n8HHCOuCN5dCw=4</t>
+          <t>+6018 1122334</t>
         </is>
       </c>
       <c r="K8" t="inlineStr">
@@ -874,14 +874,14 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>5rQfWa36yXSeJN5dTsK3K0oSNjvoD_0_ZvX7OGqZxN0=h</t>
+          <t>Priya Ramesh</t>
         </is>
       </c>
       <c r="B9" t="inlineStr"/>
       <c r="C9" t="inlineStr"/>
       <c r="D9" t="inlineStr">
         <is>
-          <t>59nG5DKQFp73BvlaUWhm7HQ_qg9bwXqM8U6gs4R7vlc=7</t>
+          <t>010909-11-4567</t>
         </is>
       </c>
       <c r="E9" t="inlineStr"/>
@@ -902,12 +902,12 @@
       </c>
       <c r="I9" t="inlineStr">
         <is>
-          <t>NuEaFj5LFIQD95_2x97bXs3gGmatVIcJ-nCZeaR67HAYPoBZ-hRZzKwSw53WVaeWm</t>
+          <t>priya.ramesh@live.com</t>
         </is>
       </c>
       <c r="J9" t="inlineStr">
         <is>
-          <t>FAReA_bPmctj7wxwoyYDIT_XBK4bPypjchi_Lss6zt4=5</t>
+          <t>010 2233445</t>
         </is>
       </c>
       <c r="K9" t="inlineStr">
@@ -927,7 +927,7 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>yz_Bt5NLkcVoAxWwJRsAI-DknmLPbnBFWMlGQibD3T0=g</t>
+          <t>Chen Xiao Long</t>
         </is>
       </c>
       <c r="B10" t="inlineStr"/>
@@ -935,7 +935,7 @@
       <c r="D10" t="inlineStr"/>
       <c r="E10" t="inlineStr">
         <is>
-          <t>srF8emOsOLHr6e-lAHrIZuc0CWCUfgRF1bLwHRC-uTg=2</t>
+          <t>E98765432</t>
         </is>
       </c>
       <c r="F10" t="inlineStr">
@@ -955,12 +955,12 @@
       </c>
       <c r="I10" t="inlineStr">
         <is>
-          <t>jK1JEge1X9kUIK7qE97XLz2NKtpbpVVhg5RcYmZDG7k0Njp2TJZwbBTGiy0n4rB4m</t>
+          <t>xiaolong.chen@china.com</t>
         </is>
       </c>
       <c r="J10" t="inlineStr">
         <is>
-          <t>i0jtxbh3OY6qKQXZIWL6UEOatz1traoXGYHJrTaLZRY=7</t>
+          <t>+6011 44556677</t>
         </is>
       </c>
       <c r="K10" t="inlineStr">
@@ -980,7 +980,7 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>LN5py1hCnDV0U9x2nGaubfkl5mBD2VEy_wfCIN4ChUs=z</t>
+          <t>Maria Gonzalez</t>
         </is>
       </c>
       <c r="B11" t="inlineStr"/>
@@ -988,7 +988,7 @@
       <c r="D11" t="inlineStr"/>
       <c r="E11" t="inlineStr">
         <is>
-          <t>r-ouB4aL6dDRxnSdltUVQNv8jLCzulndZuaD1mHfhKs=1</t>
+          <t>P87654321</t>
         </is>
       </c>
       <c r="F11" t="inlineStr">
@@ -1008,12 +1008,12 @@
       </c>
       <c r="I11" t="inlineStr">
         <is>
-          <t>6x2Xz6Gz4yvFLFlvV3VVGjTBfXzbkwGLtTU1jvJLUXqLHXgCrnubBf-1kNc9l1YYs</t>
+          <t>maria.gonzalez@espanol.es</t>
         </is>
       </c>
       <c r="J11" t="inlineStr">
         <is>
-          <t>t6R-pZ0sjIGC9hiHLYwGy3N86Jjx7NPEYPUgqtKK7IA=5</t>
+          <t>+6019 8877665</t>
         </is>
       </c>
       <c r="K11" t="inlineStr">
@@ -1033,7 +1033,7 @@
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>1bbsY1EqgVHAmtkSH1TpojHZOXv6Mws6xara2F3L_nYu_8SM3CP68GWLWDQlfaPOl</t>
+          <t>Ahmad Zulkifli bin Ismail</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
@@ -1048,7 +1048,7 @@
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>bu3bNUG9IUJbJYvO_vaaBuIBVbCq1riBn4QIFwOZAbg=5</t>
+          <t>901225-14-1235</t>
         </is>
       </c>
       <c r="E12" t="inlineStr"/>
@@ -1057,12 +1057,12 @@
       <c r="H12" t="inlineStr"/>
       <c r="I12" t="inlineStr">
         <is>
-          <t>F8ANYzbH-xqoJF8e-Y6gxOX4kZkSwGt8MKMt9pr9tjuJsRtr4GgnnQxkHzxAgIGy3zpmTMbu2Rq9GPn8uaRWUQ==m</t>
+          <t>ahmad.zulkifli..ismail51@gmail.com</t>
         </is>
       </c>
       <c r="J12" t="inlineStr">
         <is>
-          <t>JiZhMHHRq-R4Fxss96kfn-Ye43FLxrfEhsm7m4i0Y0Y=1</t>
+          <t>011-3025021</t>
         </is>
       </c>
       <c r="K12" t="inlineStr">
@@ -1082,7 +1082,7 @@
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>HtJb1bDalCJE5Li7AZUFJluh4ARZQeQauGQS02ZCs3r1yMDCHNUTRfCq6YI2VVgTn</t>
+          <t>Nur Aisyah binti Rahman</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
@@ -1097,7 +1097,7 @@
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>aeUHjUnBKaCEAMjON_-piBsIv2TRnuXrfVEFQy5PblU=8</t>
+          <t>980430-14-2468</t>
         </is>
       </c>
       <c r="E13" t="inlineStr"/>
@@ -1106,7 +1106,7 @@
       <c r="H13" t="inlineStr"/>
       <c r="I13" t="inlineStr">
         <is>
-          <t>g2K0xnbITQcpy8nahMxlVrykx7I1jqX4R1H6u-BN_znjwsu57T0a0mTiLMJVAKkom</t>
+          <t>nur.aisyah.ti.rahman71@mail.com</t>
         </is>
       </c>
       <c r="J13" t="inlineStr"/>
@@ -1127,7 +1127,7 @@
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>gfvV5ke9t1JBFmXwUlxmggotaplVqEEH3EN5H5GwUjQ=g</t>
+          <t>Lim Wei Cheng</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
@@ -1142,7 +1142,7 @@
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>-hdVzdGEh3tQ19frfUsuGeq2PRS85XaYq_SpgbctCMA=3</t>
+          <t>920101-08-1123</t>
         </is>
       </c>
       <c r="E14" t="inlineStr"/>
@@ -1151,7 +1151,7 @@
       <c r="H14" t="inlineStr"/>
       <c r="I14" t="inlineStr">
         <is>
-          <t>yf_SqPQ35rUzYz44tbO0Sr0fk-8G5OwNEO7M_aACGADGRNnW_HiUxldS8Y06EkOSm</t>
+          <t>lim.wei.cheng74@yahoo.com</t>
         </is>
       </c>
       <c r="J14" t="inlineStr"/>
@@ -1172,7 +1172,7 @@
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>KaE0uZawNAlv9XuG29gBzjDWWQwF-1-A5RD7tiwqxxk=g</t>
+          <t>Tan Mei Ling</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
@@ -1187,7 +1187,7 @@
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>Vqdm0plbXkdb2W3OCzokAGaJV6jmoal4dGbBgLonNpA=6</t>
+          <t>950715-10-2386</t>
         </is>
       </c>
       <c r="E15" t="inlineStr"/>
@@ -1196,7 +1196,7 @@
       <c r="H15" t="inlineStr"/>
       <c r="I15" t="inlineStr">
         <is>
-          <t>2TBXGwxnUiIP1H5hvngH0b7OFZSMd0ChPO2eB8cCW7D0AaE_6cHSbp1hScBd43onm</t>
+          <t>tan.mei.ling7@yahoo.com</t>
         </is>
       </c>
       <c r="J15" t="inlineStr"/>
@@ -1217,7 +1217,7 @@
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>wvcwq3j8yMfhsVLmfxjx2ZgNKbizrqxJmA6w22KYpI9DQv0yIwohm0HNawNXNMrYy</t>
+          <t>Rajesh a/l Muniandy</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
@@ -1232,7 +1232,7 @@
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>XTFL9gLu_YQIxVifoKeOAlydqf0cZRvAGws8wdJ2CPY=1</t>
+          <t>890915-04-7781</t>
         </is>
       </c>
       <c r="E16" t="inlineStr"/>
@@ -1241,7 +1241,7 @@
       <c r="H16" t="inlineStr"/>
       <c r="I16" t="inlineStr">
         <is>
-          <t>nIwGPvu8CcYCEC6fJllJvE5tHveaV1Nr2jI7zkceMfBUigU8YfeAtO3nWeJ_XPO_m</t>
+          <t>rajesh.al.muniandy86@gmail.com</t>
         </is>
       </c>
       <c r="J16" t="inlineStr"/>
@@ -1262,7 +1262,7 @@
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>DoP-OP0cvZ7LGYH_2KOH679yA8uHrY1VdrIuT4qHTuKd03veOI26_pc1y4aNf3dYm</t>
+          <t>Priya a/p Subramaniam</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
@@ -1277,7 +1277,7 @@
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>AdFEpUv22jDZEdzBTpxLH20pDu1evjYlPN8vZyiEsak=2</t>
+          <t>970312-06-4452</t>
         </is>
       </c>
       <c r="E17" t="inlineStr"/>
@@ -1286,7 +1286,7 @@
       <c r="H17" t="inlineStr"/>
       <c r="I17" t="inlineStr">
         <is>
-          <t>bmbsYo-i6heaW7AaOqvLEW27Lgadyh8OllbJvWgLa9fpTPFzmVLP5zhGDg36kyCpm</t>
+          <t>priya.ap.subramaniam11@gmail.com</t>
         </is>
       </c>
       <c r="J17" t="inlineStr"/>
@@ -1307,7 +1307,7 @@
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>IiHVclDpqMGdAnB7yjv0lRhknqZtOu3Yy5fPTdfTB90=h</t>
+          <t>Balvinder Singh</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
@@ -1322,7 +1322,7 @@
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>ct_65JGvfiiRcGqPrHpckF1TKZvI_5cDMhVyBC8Px1g=3</t>
+          <t>880101-10-8893</t>
         </is>
       </c>
       <c r="E18" t="inlineStr"/>
@@ -1331,7 +1331,7 @@
       <c r="H18" t="inlineStr"/>
       <c r="I18" t="inlineStr">
         <is>
-          <t>cGUEU-vCoeGZVJg2Wh507V-1TitTiTsXajICE_8g-Ni6t0dYFNV2cPIUwt4jDXbGm</t>
+          <t>balvinder.singh91@mail.com</t>
         </is>
       </c>
       <c r="J18" t="inlineStr"/>
@@ -1352,7 +1352,7 @@
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>-40kx0b_LjRSJxv5eoXJaSqKT5pFkMn5cNpw1FAcjvI=r</t>
+          <t>Kavitha Kaur</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
@@ -1367,7 +1367,7 @@
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>C-7npUj87XxUQzDvcSg0lLFOp2WYdlmt_sLLEzUhUco=2</t>
+          <t>910721-10-4482</t>
         </is>
       </c>
       <c r="E19" t="inlineStr"/>
@@ -1376,7 +1376,7 @@
       <c r="H19" t="inlineStr"/>
       <c r="I19" t="inlineStr">
         <is>
-          <t>dYPfJXL_ENFXIxIknmI1yfYB0uvAVIAVI_lzIXVQDar5GfkbTNzAjCaAQ05Jq0Yam</t>
+          <t>kavitha.kaur32@gmail.com</t>
         </is>
       </c>
       <c r="J19" t="inlineStr"/>
@@ -1397,7 +1397,7 @@
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>ZfaCOMgs4b-aunYp81xUG4VYkwr2ga7nHWbybLJ4dtVZAakL1q7WZVI4B5uPYIvpn</t>
+          <t>Julius anak Langkan</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
@@ -1412,7 +1412,7 @@
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>F8s55tYej38QQetZq3ZEzvlr5yCUqLdp__OtPt-ZqyU=1</t>
+          <t>900707-13-2291</t>
         </is>
       </c>
       <c r="E20" t="inlineStr"/>
@@ -1421,7 +1421,7 @@
       <c r="H20" t="inlineStr"/>
       <c r="I20" t="inlineStr">
         <is>
-          <t>twI2ukKwOGRDAV_kysQb14Bf8_V1hZScvPLvM4V2ja7gbSIOXd7_L6aRmUMHXVqDm</t>
+          <t>julius..langkan37@outlook.com</t>
         </is>
       </c>
       <c r="J20" t="inlineStr"/>
@@ -1442,7 +1442,7 @@
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>LmkMnHhjQajo5oHvaowjI-ELwLiRDqyx5EXRFnwdz5Cavamm3vZoaZpFW9nMYrUFn</t>
+          <t>Mariam binti Jaupin</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
@@ -1457,7 +1457,7 @@
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>9O-e-Q0is-noQiVdhPTWwzoQ_IACzuZj9TjafxWZPB4=8</t>
+          <t>920312-12-6458</t>
         </is>
       </c>
       <c r="E21" t="inlineStr"/>
@@ -1466,7 +1466,7 @@
       <c r="H21" t="inlineStr"/>
       <c r="I21" t="inlineStr">
         <is>
-          <t>sWa-kCYXw8snyBLGsJT5rLH3snT7d2rVnzA1M9LtjvBu3f0CUsK09h22TlUIYZ5lm</t>
+          <t>mariam.ti.jaupin72@gmail.com</t>
         </is>
       </c>
       <c r="J21" t="inlineStr"/>
@@ -1487,7 +1487,7 @@
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>AqPPNYWReqGMYpMVbkE1a7Q7iSCHsqZjNm-B58XB_ZI=z</t>
+          <t>Andrew Fernandez</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
@@ -1502,7 +1502,7 @@
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>ZC2HBNuA7zQ9Js6oCVsHq-H-2Gb_Z1YGJsvStRLMzl4=1</t>
+          <t>850928-14-5561</t>
         </is>
       </c>
       <c r="E22" t="inlineStr"/>
@@ -1511,7 +1511,7 @@
       <c r="H22" t="inlineStr"/>
       <c r="I22" t="inlineStr">
         <is>
-          <t>FKMjMh4UQRW-5SwLwZ_jYUQbTCAdE-SwsKiZyeeYZaWW9IAH16Il4n4qBcZMJGmRm</t>
+          <t>andrew.fernandez57@gmail.com</t>
         </is>
       </c>
       <c r="J22" t="inlineStr"/>
@@ -1532,7 +1532,7 @@
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>M3-hUBs9y_lyHosczPuyDae_nKjydzXkYOvgcipsG00=t</t>
+          <t>Niran Prasert</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
@@ -1547,7 +1547,7 @@
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>YpQitkOowBSEwtAYuo4TKM5_9Zj6Z83KraHtuku5KOA=1</t>
+          <t>890614-09-3381</t>
         </is>
       </c>
       <c r="E23" t="inlineStr"/>
@@ -1556,12 +1556,12 @@
       <c r="H23" t="inlineStr"/>
       <c r="I23" t="inlineStr">
         <is>
-          <t>m93EjyBmZTHJ8t6L6OlXdv5mxWzXFCS_mbJMb06W9qt8kLgKlFpMDXmGhfzOj4C0m</t>
+          <t>niran.prasert56@gmail.com</t>
         </is>
       </c>
       <c r="J23" t="inlineStr">
         <is>
-          <t>YoKfw0RaZrLUWHcGSY-TyaRpjDrv4TOOFUmMOIMnN3E=5</t>
+          <t>015-7639065</t>
         </is>
       </c>
       <c r="K23" t="inlineStr">

</xml_diff>